<commit_message>
Append to Report-2025-05-05.xlsx at ٠٥‏/٠٥‏/٢٠٢٥ ٠١:٥٩:١٤ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-05.xlsx
+++ b/Database/Report-2025-05-05.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -454,9 +454,35 @@
         <v>٠٥‏/٠٥‏/٢٠٢٥ ٠١:٥٩:٠٨ م</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C3" t="str">
+        <v>233</v>
+      </c>
+      <c r="D3" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E3" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F3" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G3" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H3" t="str">
+        <v>٠٥‏/٠٥‏/٢٠٢٥ ٠١:٥٩:١٤ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-05.xlsx at ٠٥‏/٠٥‏/٢٠٢٥ ٠٢:٠١:٢٠ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-05.xlsx
+++ b/Database/Report-2025-05-05.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,9 +480,35 @@
         <v>٠٥‏/٠٥‏/٢٠٢٥ ٠١:٥٩:١٤ م</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C4" t="str">
+        <v>233</v>
+      </c>
+      <c r="D4" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E4" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F4" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G4" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H4" t="str">
+        <v>٠٥‏/٠٥‏/٢٠٢٥ ٠٢:٠١:٢٠ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-05.xlsx at ٠٥‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٢٩ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-05.xlsx
+++ b/Database/Report-2025-05-05.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -506,9 +506,35 @@
         <v>٠٥‏/٠٥‏/٢٠٢٥ ٠٢:٠١:٢٠ م</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C5" t="str">
+        <v>233</v>
+      </c>
+      <c r="D5" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E5" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F5" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G5" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H5" t="str">
+        <v>٠٥‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٢٩ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Append to Report-2025-05-05.xlsx at ٠٥‏/٠٥‏/٢٠٢٥ ٠٢:٢٧:١٧ م
</commit_message>
<xml_diff>
--- a/Database/Report-2025-05-05.xlsx
+++ b/Database/Report-2025-05-05.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,9 +532,35 @@
         <v>٠٥‏/٠٥‏/٢٠٢٥ ٠٢:١٠:٢٩ م</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v/>
+      </c>
+      <c r="B6" t="str">
+        <v>احمد</v>
+      </c>
+      <c r="C6" t="str">
+        <v>233</v>
+      </c>
+      <c r="D6" t="str">
+        <v>الصمود</v>
+      </c>
+      <c r="E6" t="str">
+        <v>الرحلة 2</v>
+      </c>
+      <c r="F6" t="str">
+        <v>C2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>IDRF</v>
+      </c>
+      <c r="H6" t="str">
+        <v>٠٥‏/٠٥‏/٢٠٢٥ ٠٢:٢٧:١٧ م</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>